<commit_message>
GUI, helper functions separate file and raw_correlations changes
</commit_message>
<xml_diff>
--- a/Progress dataframes/raw_correlations/output_df_corrections.xlsx
+++ b/Progress dataframes/raw_correlations/output_df_corrections.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_current\NPSoftware\GitHub\Progress dataframes\raw_correlations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A558E083-3AF4-4BCE-BCF8-E39654B014F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -73,8 +79,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +143,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -183,7 +197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,9 +229,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,6 +281,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,14 +474,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -468,25 +520,25 @@
         <v>9</v>
       </c>
       <c r="D2">
-        <v>0.4426341946409725</v>
+        <v>0.44263419464097248</v>
       </c>
       <c r="E2">
-        <v>0.3692770409224844</v>
+        <v>0.36927704092248442</v>
       </c>
       <c r="F2">
-        <v>0.5105094338403686</v>
+        <v>0.51050943384036862</v>
       </c>
       <c r="G2">
-        <v>2.100907740278534e-25</v>
+        <v>2.1009077402785341E-25</v>
       </c>
       <c r="H2">
-        <v>9.804236121299825e-25</v>
+        <v>9.8042361212998251E-25</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -503,19 +555,19 @@
         <v>0.1730646254663579</v>
       </c>
       <c r="F3">
-        <v>0.3369580743248051</v>
+        <v>0.33695807432480512</v>
       </c>
       <c r="G3">
-        <v>5.637473112054037e-09</v>
+        <v>5.6374731120540371E-9</v>
       </c>
       <c r="H3">
-        <v>1.57849247137513e-08</v>
+        <v>1.5784924713751302E-8</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -526,25 +578,25 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>0.2167213575424491</v>
+        <v>0.21672135754244909</v>
       </c>
       <c r="E4">
-        <v>0.1315304298495431</v>
+        <v>0.13153042984954311</v>
       </c>
       <c r="F4">
         <v>0.2987346651864865</v>
       </c>
       <c r="G4">
-        <v>9.973077661020257e-07</v>
+        <v>9.9730776610202572E-7</v>
       </c>
       <c r="H4">
-        <v>2.53860158644152e-06</v>
+        <v>2.5386015864415199E-6</v>
       </c>
       <c r="I4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -555,25 +607,25 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>0.3273714559640772</v>
+        <v>0.32737145596407718</v>
       </c>
       <c r="E5">
-        <v>0.2467648442620183</v>
+        <v>0.24676484426201831</v>
       </c>
       <c r="F5">
-        <v>0.4034792065117352</v>
+        <v>0.40347920651173519</v>
       </c>
       <c r="G5">
-        <v>5.919468232961133e-14</v>
+        <v>5.9194682329611331E-14</v>
       </c>
       <c r="H5">
-        <v>2.367787293184453e-13</v>
+        <v>2.3677872931844532E-13</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -584,25 +636,25 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>-0.06537285585059048</v>
+        <v>-6.5372855850590481E-2</v>
       </c>
       <c r="E6">
-        <v>-0.1521909958061347</v>
+        <v>-0.15219099580613471</v>
       </c>
       <c r="F6">
-        <v>0.02244640771560838</v>
+        <v>2.244640771560838E-2</v>
       </c>
       <c r="G6">
-        <v>0.1443767841581503</v>
+        <v>0.14437678415815031</v>
       </c>
       <c r="H6">
-        <v>0.2245861086904561</v>
+        <v>0.22458610869045609</v>
       </c>
       <c r="I6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -613,25 +665,25 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>0.080130450419095</v>
+        <v>8.0130450419095001E-2</v>
       </c>
       <c r="E7">
-        <v>-0.007613635856765775</v>
+        <v>-7.6136358567657752E-3</v>
       </c>
       <c r="F7">
-        <v>0.166650040510163</v>
+        <v>0.16665004051016299</v>
       </c>
       <c r="G7">
-        <v>0.07342718919439439</v>
+        <v>7.3427189194394393E-2</v>
       </c>
       <c r="H7">
-        <v>0.1284975810901902</v>
+        <v>0.12849758109019019</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -642,10 +694,10 @@
         <v>15</v>
       </c>
       <c r="D8">
-        <v>0.06971480660622964</v>
+        <v>6.971480660622964E-2</v>
       </c>
       <c r="E8">
-        <v>-0.01808634890096351</v>
+        <v>-1.8086348900963511E-2</v>
       </c>
       <c r="F8">
         <v>0.1564489697024386</v>
@@ -654,13 +706,13 @@
         <v>0.1195029079426661</v>
       </c>
       <c r="H8">
-        <v>0.1968283189643913</v>
+        <v>0.19682831896439129</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -671,25 +723,25 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>0.2594528647353534</v>
+        <v>0.25945286473535339</v>
       </c>
       <c r="E9">
         <v>0.1757611192314025</v>
       </c>
       <c r="F9">
-        <v>0.3394210883132802</v>
+        <v>0.33942108831328022</v>
       </c>
       <c r="G9">
-        <v>3.905448357083225e-09</v>
+        <v>3.9054483570832252E-9</v>
       </c>
       <c r="H9">
-        <v>1.215028377759226e-08</v>
+        <v>1.215028377759226E-8</v>
       </c>
       <c r="I9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -706,19 +758,19 @@
         <v>0.1214704283688324</v>
       </c>
       <c r="F10">
-        <v>0.2893951567637653</v>
+        <v>0.28939515676376532</v>
       </c>
       <c r="G10">
-        <v>3.060396135206066e-06</v>
+        <v>3.0603961352060662E-6</v>
       </c>
       <c r="H10">
-        <v>7.140924315480821e-06</v>
+        <v>7.1409243154808207E-6</v>
       </c>
       <c r="I10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -729,25 +781,25 @@
         <v>12</v>
       </c>
       <c r="D11">
-        <v>0.3098152618048072</v>
+        <v>0.30981526180480717</v>
       </c>
       <c r="E11">
-        <v>0.2283278585626257</v>
+        <v>0.22832785856262569</v>
       </c>
       <c r="F11">
-        <v>0.3869920937687237</v>
+        <v>0.38699209376872368</v>
       </c>
       <c r="G11">
-        <v>1.386277660994235e-12</v>
+        <v>1.3862776609942349E-12</v>
       </c>
       <c r="H11">
-        <v>4.851971813479821e-12</v>
+        <v>4.8519718134798207E-12</v>
       </c>
       <c r="I11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -758,25 +810,25 @@
         <v>13</v>
       </c>
       <c r="D12">
-        <v>-0.05698052561971693</v>
+        <v>-5.6980525619716928E-2</v>
       </c>
       <c r="E12">
-        <v>-0.1439518354946406</v>
+        <v>-0.14395183549464061</v>
       </c>
       <c r="F12">
-        <v>0.03086428020946452</v>
+        <v>3.086428020946452E-2</v>
       </c>
       <c r="G12">
-        <v>0.2033845210195596</v>
+        <v>0.20338452101955959</v>
       </c>
       <c r="H12">
-        <v>0.2711793613594128</v>
+        <v>0.27117936135941278</v>
       </c>
       <c r="I12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -787,25 +839,25 @@
         <v>14</v>
       </c>
       <c r="D13">
-        <v>0.06047622204977514</v>
+        <v>6.0476222049775138E-2</v>
       </c>
       <c r="E13">
-        <v>-0.02735945814940322</v>
+        <v>-2.7359458149403219E-2</v>
       </c>
       <c r="F13">
         <v>0.1473851971878386</v>
       </c>
       <c r="G13">
-        <v>0.1769708121491199</v>
+        <v>0.17697081214911989</v>
       </c>
       <c r="H13">
-        <v>0.257592280128522</v>
+        <v>0.25759228012852198</v>
       </c>
       <c r="I13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -816,25 +868,25 @@
         <v>15</v>
       </c>
       <c r="D14">
-        <v>0.1476670352568653</v>
+        <v>0.14766703525686531</v>
       </c>
       <c r="E14">
-        <v>0.06076327177061379</v>
+        <v>6.0763271770613789E-2</v>
       </c>
       <c r="F14">
-        <v>0.232348934436259</v>
+        <v>0.23234893443625901</v>
       </c>
       <c r="G14">
-        <v>0.0009268310955008412</v>
+        <v>9.2683109550084121E-4</v>
       </c>
       <c r="H14">
-        <v>0.001996251590309504</v>
+        <v>1.9962515903095041E-3</v>
       </c>
       <c r="I14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -845,25 +897,25 @@
         <v>11</v>
       </c>
       <c r="D15">
-        <v>0.0326052984477787</v>
+        <v>3.2605298447778701E-2</v>
       </c>
       <c r="E15">
-        <v>-0.05524323944019509</v>
+        <v>-5.5243239440195088E-2</v>
       </c>
       <c r="F15">
-        <v>0.1199529193711218</v>
+        <v>0.11995291937112181</v>
       </c>
       <c r="G15">
-        <v>0.4669532275051859</v>
+        <v>0.46695322750518592</v>
       </c>
       <c r="H15">
-        <v>0.5447787654227169</v>
+        <v>0.54477876542271686</v>
       </c>
       <c r="I15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -874,25 +926,25 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <v>0.7035147692814612</v>
+        <v>0.70351476928146117</v>
       </c>
       <c r="E16">
-        <v>0.656313209050279</v>
+        <v>0.65631320905027901</v>
       </c>
       <c r="F16">
-        <v>0.7452308555397629</v>
+        <v>0.74523085553976287</v>
       </c>
       <c r="G16">
-        <v>6.899936297513961e-76</v>
+        <v>6.8999362975139607E-76</v>
       </c>
       <c r="H16">
-        <v>6.439940544346363e-75</v>
+        <v>6.4399405443463633E-75</v>
       </c>
       <c r="I16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -903,25 +955,25 @@
         <v>13</v>
       </c>
       <c r="D17">
-        <v>-0.7486305582816598</v>
+        <v>-0.74863055828165981</v>
       </c>
       <c r="E17">
-        <v>-0.7848006666681215</v>
+        <v>-0.78480066666812154</v>
       </c>
       <c r="F17">
-        <v>-0.7073778052229214</v>
+        <v>-0.70737780522292137</v>
       </c>
       <c r="G17">
-        <v>6.134607085875902e-91</v>
+        <v>6.1346070858759022E-91</v>
       </c>
       <c r="H17">
-        <v>8.588449920226264e-90</v>
+        <v>8.5884499202262638E-90</v>
       </c>
       <c r="I17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -932,16 +984,16 @@
         <v>14</v>
       </c>
       <c r="D18">
-        <v>0.0422591876465824</v>
+        <v>4.2259187646582402E-2</v>
       </c>
       <c r="E18">
-        <v>-0.04560038284204614</v>
+        <v>-4.5600382842046143E-2</v>
       </c>
       <c r="F18">
         <v>0.1294699940625193</v>
       </c>
       <c r="G18">
-        <v>0.3456807077729216</v>
+        <v>0.34568070777292159</v>
       </c>
       <c r="H18">
         <v>0.4208286877235568</v>
@@ -950,7 +1002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -961,25 +1013,25 @@
         <v>15</v>
       </c>
       <c r="D19">
-        <v>0.006724955670680418</v>
+        <v>6.7249556706804178E-3</v>
       </c>
       <c r="E19">
-        <v>-0.08101340682121708</v>
+        <v>-8.1013406821217077E-2</v>
       </c>
       <c r="F19">
-        <v>0.09435989783903898</v>
+        <v>9.4359897839038975E-2</v>
       </c>
       <c r="G19">
-        <v>0.8807646887707907</v>
+        <v>0.88076468877079073</v>
       </c>
       <c r="H19">
-        <v>0.8807646887707907</v>
+        <v>0.88076468877079073</v>
       </c>
       <c r="I19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -990,25 +1042,25 @@
         <v>12</v>
       </c>
       <c r="D20">
-        <v>0.6879360801900264</v>
+        <v>0.68793608019002639</v>
       </c>
       <c r="E20">
-        <v>0.6387802422725878</v>
+        <v>0.63878024227258778</v>
       </c>
       <c r="F20">
-        <v>0.7314986330504997</v>
+        <v>0.73149863305049967</v>
       </c>
       <c r="G20">
-        <v>2.471082338397796e-71</v>
+        <v>2.4710823383977958E-71</v>
       </c>
       <c r="H20">
-        <v>1.729757636878458e-70</v>
+        <v>1.7297576368784579E-70</v>
       </c>
       <c r="I20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1019,25 +1071,25 @@
         <v>13</v>
       </c>
       <c r="D21">
-        <v>0.5965884118495778</v>
+        <v>0.59658841184957778</v>
       </c>
       <c r="E21">
-        <v>0.5369905879936365</v>
+        <v>0.53699058799363653</v>
       </c>
       <c r="F21">
-        <v>0.6502604989707295</v>
+        <v>0.65026049897072946</v>
       </c>
       <c r="G21">
-        <v>1.59319460724825e-49</v>
+        <v>1.59319460724825E-49</v>
       </c>
       <c r="H21">
-        <v>8.921889800590201e-49</v>
+        <v>8.9218898005902013E-49</v>
       </c>
       <c r="I21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1048,16 +1100,16 @@
         <v>14</v>
       </c>
       <c r="D22">
-        <v>0.08504545331960232</v>
+        <v>8.5045453319602324E-2</v>
       </c>
       <c r="E22">
-        <v>-0.002665009126260277</v>
+        <v>-2.6650091262602768E-3</v>
       </c>
       <c r="F22">
         <v>0.1714573658062731</v>
       </c>
       <c r="G22">
-        <v>0.05738608487990657</v>
+        <v>5.7386084879906568E-2</v>
       </c>
       <c r="H22">
         <v>0.1071206917758256</v>
@@ -1066,7 +1118,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1077,25 +1129,25 @@
         <v>15</v>
       </c>
       <c r="D23">
-        <v>0.04819183207613009</v>
+        <v>4.8191832076130092E-2</v>
       </c>
       <c r="E23">
-        <v>-0.03966638452302909</v>
+        <v>-3.9666384523029091E-2</v>
       </c>
       <c r="F23">
         <v>0.1353106011700321</v>
       </c>
       <c r="G23">
-        <v>0.2821375037599094</v>
+        <v>0.28213750375990942</v>
       </c>
       <c r="H23">
-        <v>0.3590840956944302</v>
+        <v>0.35908409569443023</v>
       </c>
       <c r="I23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1106,25 +1158,25 @@
         <v>13</v>
       </c>
       <c r="D24">
-        <v>-0.1318403511667668</v>
+        <v>-0.13184035116676679</v>
       </c>
       <c r="E24">
         <v>-0.217021914200826</v>
       </c>
       <c r="F24">
-        <v>-0.04466615600251755</v>
+        <v>-4.4666156002517547E-2</v>
       </c>
       <c r="G24">
-        <v>0.003141277276814314</v>
+        <v>3.1412772768143141E-3</v>
       </c>
       <c r="H24">
-        <v>0.006282554553628627</v>
+        <v>6.2825545536286274E-3</v>
       </c>
       <c r="I24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1135,25 +1187,25 @@
         <v>14</v>
       </c>
       <c r="D25">
-        <v>0.05951111250263295</v>
+        <v>5.9511112502632947E-2</v>
       </c>
       <c r="E25">
-        <v>-0.02832730299830354</v>
+        <v>-2.8327302998303539E-2</v>
       </c>
       <c r="F25">
-        <v>0.1464375065852246</v>
+        <v>0.14643750658522461</v>
       </c>
       <c r="G25">
-        <v>0.1839944858060872</v>
+        <v>0.18399448580608721</v>
       </c>
       <c r="H25">
-        <v>0.257592280128522</v>
+        <v>0.25759228012852198</v>
       </c>
       <c r="I25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1164,25 +1216,25 @@
         <v>15</v>
       </c>
       <c r="D26">
-        <v>0.01601933374192419</v>
+        <v>1.6019333741924189E-2</v>
       </c>
       <c r="E26">
-        <v>-0.07177207535216241</v>
+        <v>-7.1772075352162415E-2</v>
       </c>
       <c r="F26">
         <v>0.1035644397799674</v>
       </c>
       <c r="G26">
-        <v>0.7208450866116068</v>
+        <v>0.72084508661160684</v>
       </c>
       <c r="H26">
-        <v>0.7509745471757853</v>
+        <v>0.75097454717578527</v>
       </c>
       <c r="I26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1193,25 +1245,25 @@
         <v>14</v>
       </c>
       <c r="D27">
-        <v>0.01602687983379825</v>
+        <v>1.602687983379825E-2</v>
       </c>
       <c r="E27">
-        <v>-0.07176456619998303</v>
+        <v>-7.1764566199983032E-2</v>
       </c>
       <c r="F27">
         <v>0.1035719068467886</v>
       </c>
       <c r="G27">
-        <v>0.7207190771758407</v>
+        <v>0.72071907717584072</v>
       </c>
       <c r="H27">
-        <v>0.7509745471757853</v>
+        <v>0.75097454717578527</v>
       </c>
       <c r="I27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1222,10 +1274,10 @@
         <v>15</v>
       </c>
       <c r="D28">
-        <v>0.01582133853089687</v>
+        <v>1.5821338530896869E-2</v>
       </c>
       <c r="E28">
-        <v>-0.0719690977791704</v>
+        <v>-7.1969097779170405E-2</v>
       </c>
       <c r="F28">
         <v>0.1033685145107964</v>
@@ -1234,13 +1286,13 @@
         <v>0.724154027633793</v>
       </c>
       <c r="H28">
-        <v>0.7509745471757853</v>
+        <v>0.75097454717578527</v>
       </c>
       <c r="I28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1251,19 +1303,19 @@
         <v>15</v>
       </c>
       <c r="D29">
-        <v>0.7598726488807575</v>
+        <v>0.75987264888075745</v>
       </c>
       <c r="E29">
-        <v>0.720169612075601</v>
+        <v>0.72016961207560104</v>
       </c>
       <c r="F29">
-        <v>0.7946151083739481</v>
+        <v>0.79461510837394811</v>
       </c>
       <c r="G29">
-        <v>3.361462316991158e-95</v>
+        <v>3.3614623169911581E-95</v>
       </c>
       <c r="H29">
-        <v>9.412094487575243e-94</v>
+        <v>9.4120944875752432E-94</v>
       </c>
       <c r="I29" t="s">
         <v>16</v>

</xml_diff>